<commit_message>
Added NUnit tests to project based on Excel Added Excel file with 2-4
</commit_message>
<xml_diff>
--- a/Other Files/Tests + FlowGraph.xlsx
+++ b/Other Files/Tests + FlowGraph.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marty\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marty\Documents\Development\SQTAssignment\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -121,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -129,13 +129,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3143,10 +3221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H5:O18"/>
+  <dimension ref="H4:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3156,26 +3234,27 @@
     <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="8:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="8:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I5">
         <v>22</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3186,14 +3265,20 @@
       <c r="I6">
         <v>16</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="8:15" x14ac:dyDescent="0.25">
@@ -3203,71 +3288,147 @@
       <c r="I7">
         <v>8</v>
       </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="K8">
+      <c r="K8" s="2">
         <v>2</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="N8" s="2">
+        <v>6</v>
+      </c>
+      <c r="O8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="K10">
+      <c r="K10" s="2">
         <v>3</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="N10" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="11" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
     </row>
     <row r="12" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="K12">
+      <c r="K12" s="2">
         <v>4</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="N12" s="2">
+        <v>5</v>
+      </c>
+      <c r="O12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
     </row>
     <row r="14" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="K14">
+      <c r="K14" s="2">
         <v>5</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="N14" s="2">
+        <v>5</v>
+      </c>
+      <c r="O14" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
     </row>
     <row r="16" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="K16">
+      <c r="K16" s="2">
         <v>6</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K18">
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K18" s="2">
         <v>7</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put all tests in one excel
</commit_message>
<xml_diff>
--- a/Other Files/Tests + FlowGraph.xlsx
+++ b/Other Files/Tests + FlowGraph.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Edges:</t>
   </si>
@@ -90,6 +90,75 @@
   </si>
   <si>
     <t>25, neither</t>
+  </si>
+  <si>
+    <t>"xyz"</t>
+  </si>
+  <si>
+    <t>non-numeric</t>
+  </si>
+  <si>
+    <t>50, 51</t>
+  </si>
+  <si>
+    <t>&gt;= 50</t>
+  </si>
+  <si>
+    <t>49, 50</t>
+  </si>
+  <si>
+    <t>&lt; 50</t>
+  </si>
+  <si>
+    <t>18, 35</t>
+  </si>
+  <si>
+    <t>&gt;18 &amp; &lt;=35</t>
+  </si>
+  <si>
+    <t>18, 30</t>
+  </si>
+  <si>
+    <t>&gt;18 &amp; &lt;=30</t>
+  </si>
+  <si>
+    <t>17, 18</t>
+  </si>
+  <si>
+    <t>&lt; 18</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>"female"</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>"male"</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Boundary Values</t>
+  </si>
+  <si>
+    <t>Rep Value</t>
+  </si>
+  <si>
+    <t>Equivalence Classes</t>
+  </si>
+  <si>
+    <t>Variable</t>
   </si>
 </sst>
 </file>
@@ -121,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -202,11 +271,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -214,6 +415,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2916,6 +3128,81 @@
             <a:rPr lang="en-IE" sz="1100"/>
             <a:t>100% Branch Coverage Tests</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="TextBox 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EE72842-A62A-474B-BE97-0C55E1578B42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6896100" y="3743325"/>
+          <a:ext cx="2257425" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>FitNesse</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0"/>
+            <a:t> Equivalence Partitioning</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3221,10 +3508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H4:O18"/>
+  <dimension ref="H4:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,6 +3519,7 @@
     <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="8:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3431,6 +3719,131 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="11:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K24" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N24" s="10"/>
+    </row>
+    <row r="25" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K25" s="11"/>
+      <c r="L25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="10"/>
+    </row>
+    <row r="26" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K26" s="11"/>
+      <c r="L26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="10"/>
+    </row>
+    <row r="27" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K27" s="14"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="12"/>
+    </row>
+    <row r="28" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K28" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="2">
+        <v>16</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K29" s="11"/>
+      <c r="L29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M29" s="2">
+        <v>24</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K30" s="11"/>
+      <c r="L30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30" s="2">
+        <v>31</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K31" s="11"/>
+      <c r="L31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" s="2">
+        <v>47</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K32" s="11"/>
+      <c r="L32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="2">
+        <v>55</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K33" s="9"/>
+      <c r="L33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>